<commit_message>
[FIX][V_2.91] Added a new row in the parsing table to allow declaration and assignation of variables
</commit_message>
<xml_diff>
--- a/ParsingTableXLSX.xlsx
+++ b/ParsingTableXLSX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D\Desktop\Tec\8voSem\AppsAvanzadas\parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFD1959-1B24-487F-A384-CC5829F4A4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE6450C-DA6A-4FB3-8EEB-8A89DA82731B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="15720" xr2:uid="{69DFC95A-4F00-4829-9476-093E2826E66E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{69DFC95A-4F00-4829-9476-093E2826E66E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="115">
   <si>
     <t>&lt;program&gt;</t>
   </si>
@@ -269,9 +269,6 @@
     <t>'[' ']'</t>
   </si>
   <si>
-    <t>'{' &lt;local-declarations&gt; &lt;statement-list&gt; '}'</t>
-  </si>
-  <si>
     <t>&lt;var-declaration&gt; &lt;local-declarations&gt;</t>
   </si>
   <si>
@@ -366,13 +363,34 @@
   </si>
   <si>
     <t>;'</t>
+  </si>
+  <si>
+    <t>,' &lt;ID&gt; &lt;declaration-prime&gt;</t>
+  </si>
+  <si>
+    <t>{' &lt;local-declarations&gt; &lt;statement-list&gt; '}'</t>
+  </si>
+  <si>
+    <t>,' &lt;ID&gt; &lt;var-declaration-prime&gt;</t>
+  </si>
+  <si>
+    <t>=' NUM ';'</t>
+  </si>
+  <si>
+    <t>&lt;asg-declaration-prime&gt;</t>
+  </si>
+  <si>
+    <t>=' &lt;asg-declaration_prime&gt; ';'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,6 +456,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -586,10 +611,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -644,12 +670,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="32">
@@ -1194,8 +1227,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D3146D21-DD59-4405-8F52-3E1A41B34FF7}" name="Table1" displayName="Table1" ref="C4:AE44" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
-  <autoFilter ref="C4:AE44" xr:uid="{D3146D21-DD59-4405-8F52-3E1A41B34FF7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D3146D21-DD59-4405-8F52-3E1A41B34FF7}" name="Table1" displayName="Table1" ref="C4:AE45" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+  <autoFilter ref="C4:AE45" xr:uid="{D3146D21-DD59-4405-8F52-3E1A41B34FF7}"/>
   <tableColumns count="29">
     <tableColumn id="1" xr3:uid="{BA622469-78E2-4F3D-860A-43050C666B9E}" name="Non-terminals"/>
     <tableColumn id="2" xr3:uid="{54EEC06A-6559-4067-A460-CA6E11E26D41}" name="'('" dataDxfId="27"/>
@@ -1548,10 +1581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF9A23D-0ECE-44A8-B7CA-F84575C1F959}">
-  <dimension ref="B3:AF44"/>
+  <dimension ref="B3:AF45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C4" zoomScale="82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B8" zoomScale="62" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1562,7 +1595,7 @@
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" customWidth="1"/>
     <col min="10" max="10" width="16.33203125" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
     <col min="12" max="12" width="11.6640625" customWidth="1"/>
@@ -1647,7 +1680,7 @@
         <v>49</v>
       </c>
       <c r="W4" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="X4" s="16" t="s">
         <v>51</v>
@@ -1675,7 +1708,7 @@
       </c>
     </row>
     <row r="5" spans="2:32" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="23">
+      <c r="B5" s="22">
         <v>0</v>
       </c>
       <c r="C5" s="13" t="s">
@@ -1721,7 +1754,7 @@
       </c>
     </row>
     <row r="6" spans="2:32" ht="32.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="23">
+      <c r="B6" s="22">
         <v>1</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -1763,7 +1796,7 @@
       </c>
     </row>
     <row r="7" spans="2:32" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="23">
+      <c r="B7" s="22">
         <v>2</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -1803,27 +1836,31 @@
       <c r="AE7" s="9"/>
     </row>
     <row r="8" spans="2:32" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="23">
+      <c r="B8" s="22">
         <v>3</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>60</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="I8" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
+      <c r="L8" s="21" t="s">
+        <v>112</v>
+      </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
@@ -1845,7 +1882,7 @@
       <c r="AE8" s="9"/>
     </row>
     <row r="9" spans="2:32" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="23">
+      <c r="B9" s="22">
         <v>4</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -1864,10 +1901,10 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-      <c r="Q9" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="R9" s="5" t="s">
+      <c r="Q9" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="R9" s="23" t="s">
         <v>45</v>
       </c>
       <c r="S9" s="5"/>
@@ -1885,7 +1922,7 @@
       <c r="AE9" s="9"/>
     </row>
     <row r="10" spans="2:32" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="23">
+      <c r="B10" s="22">
         <v>5</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -1904,7 +1941,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
-      <c r="Q10" s="5" t="s">
+      <c r="Q10" s="24" t="s">
         <v>6</v>
       </c>
       <c r="R10" s="5" t="s">
@@ -1925,7 +1962,7 @@
       <c r="AE10" s="9"/>
     </row>
     <row r="11" spans="2:32" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="23">
+      <c r="B11" s="22">
         <v>6</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -1965,7 +2002,7 @@
       <c r="AE11" s="9"/>
     </row>
     <row r="12" spans="2:32" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="23">
+      <c r="B12" s="22">
         <v>7</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -2004,8 +2041,8 @@
       <c r="AD12" s="5"/>
       <c r="AE12" s="9"/>
     </row>
-    <row r="13" spans="2:32" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="23">
+    <row r="13" spans="2:32" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="22">
         <v>8</v>
       </c>
       <c r="C13" s="15" t="s">
@@ -2045,7 +2082,7 @@
       <c r="AE13" s="9"/>
     </row>
     <row r="14" spans="2:32" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="23">
+      <c r="B14" s="22">
         <v>9</v>
       </c>
       <c r="C14" s="14" t="s">
@@ -2087,7 +2124,7 @@
       <c r="AE14" s="9"/>
     </row>
     <row r="15" spans="2:32" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="23">
+      <c r="B15" s="22">
         <v>10</v>
       </c>
       <c r="C15" s="15" t="s">
@@ -2099,8 +2136,8 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="5" t="s">
-        <v>77</v>
+      <c r="J15" s="21" t="s">
+        <v>110</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
@@ -2125,7 +2162,7 @@
       <c r="AE15" s="9"/>
     </row>
     <row r="16" spans="2:32" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="23">
+      <c r="B16" s="22">
         <v>11</v>
       </c>
       <c r="C16" s="14" t="s">
@@ -2159,10 +2196,10 @@
         <v>59</v>
       </c>
       <c r="Q16" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
@@ -2183,7 +2220,7 @@
       <c r="AE16" s="9"/>
     </row>
     <row r="17" spans="2:31" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="23">
+      <c r="B17" s="22">
         <v>12</v>
       </c>
       <c r="C17" s="15" t="s">
@@ -2203,10 +2240,10 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R17" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
@@ -2222,11 +2259,11 @@
       <c r="AD17" s="5"/>
       <c r="AE17" s="9"/>
     </row>
-    <row r="18" spans="2:31" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="23">
+    <row r="18" spans="2:31" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="22">
         <v>13</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="15" t="s">
         <v>62</v>
       </c>
       <c r="D18" s="5"/>
@@ -2238,10 +2275,14 @@
       <c r="H18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I18" s="5"/>
+      <c r="I18" s="21" t="s">
+        <v>111</v>
+      </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+      <c r="L18" s="21" t="s">
+        <v>114</v>
+      </c>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
@@ -2262,40 +2303,26 @@
       <c r="AD18" s="5"/>
       <c r="AE18" s="9"/>
     </row>
-    <row r="19" spans="2:31" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="23">
+    <row r="19" spans="2:31" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="22">
         <v>14</v>
       </c>
-      <c r="C19" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>80</v>
-      </c>
+      <c r="C19" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="F19" s="21"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="5" t="s">
-        <v>80</v>
-      </c>
+      <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="K19" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
       <c r="L19" s="5"/>
-      <c r="M19" s="5" t="s">
-        <v>80</v>
-      </c>
+      <c r="M19" s="5"/>
       <c r="N19" s="5"/>
-      <c r="O19" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="P19" s="5" t="s">
-        <v>80</v>
-      </c>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
@@ -2309,44 +2336,46 @@
       <c r="AA19" s="5"/>
       <c r="AB19" s="5"/>
       <c r="AC19" s="5" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="AD19" s="5" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="AE19" s="9"/>
     </row>
-    <row r="20" spans="2:31" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="23">
+    <row r="20" spans="2:31" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="22">
         <v>15</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>12</v>
+      <c r="C20" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K20" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="N20" s="5"/>
       <c r="O20" s="5" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
@@ -2361,37 +2390,45 @@
       <c r="AA20" s="5"/>
       <c r="AB20" s="5"/>
       <c r="AC20" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD20" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE20" s="9"/>
+    </row>
+    <row r="21" spans="2:31" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="22">
+        <v>16</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="AD20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE20" s="9"/>
-    </row>
-    <row r="21" spans="2:31" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="23">
-        <v>16</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
+      <c r="J21" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
+      <c r="M21" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
+      <c r="O21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
@@ -2405,32 +2442,34 @@
       <c r="AA21" s="5"/>
       <c r="AB21" s="5"/>
       <c r="AC21" s="5" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="AD21" s="5" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="AE21" s="9"/>
     </row>
-    <row r="22" spans="2:31" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="23">
+    <row r="22" spans="2:31" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="22">
         <v>17</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="5"/>
+      <c r="C22" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="H22" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
-      <c r="M22" s="21" t="s">
-        <v>107</v>
-      </c>
+      <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
@@ -2446,46 +2485,36 @@
       <c r="Z22" s="5"/>
       <c r="AA22" s="5"/>
       <c r="AB22" s="5"/>
-      <c r="AC22" s="5"/>
-      <c r="AD22" s="5"/>
+      <c r="AC22" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD22" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="AE22" s="9"/>
     </row>
-    <row r="23" spans="2:31" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="23">
+    <row r="23" spans="2:31" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="22">
         <v>18</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="C23" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="H23" s="5"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="K23" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
       <c r="L23" s="5"/>
-      <c r="M23" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="N23" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="O23" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="P23" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="M23" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
       <c r="S23" s="5"/>
@@ -2498,36 +2527,46 @@
       <c r="Z23" s="5"/>
       <c r="AA23" s="5"/>
       <c r="AB23" s="5"/>
-      <c r="AC23" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD23" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="AC23" s="5"/>
+      <c r="AD23" s="5"/>
       <c r="AE23" s="9"/>
     </row>
-    <row r="24" spans="2:31" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="23">
+    <row r="24" spans="2:31" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="22">
         <v>19</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="5"/>
+      <c r="C24" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="H24" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
+      <c r="J24" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="P24" s="5"/>
+      <c r="M24" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="O24" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="P24" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
       <c r="S24" s="5"/>
@@ -2540,16 +2579,20 @@
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
       <c r="AB24" s="5"/>
-      <c r="AC24" s="5"/>
-      <c r="AD24" s="5"/>
+      <c r="AC24" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD24" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="AE24" s="9"/>
     </row>
     <row r="25" spans="2:31" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="23">
+      <c r="B25" s="22">
         <v>20</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>16</v>
+      <c r="C25" s="14" t="s">
+        <v>15</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -2562,10 +2605,10 @@
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5" t="s">
-        <v>84</v>
-      </c>
+      <c r="O25" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
@@ -2582,22 +2625,18 @@
       <c r="AD25" s="5"/>
       <c r="AE25" s="9"/>
     </row>
-    <row r="26" spans="2:31" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="23">
+    <row r="26" spans="2:31" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="22">
         <v>21</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>81</v>
-      </c>
+      <c r="C26" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="5" t="s">
-        <v>85</v>
-      </c>
+      <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -2605,7 +2644,9 @@
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
+      <c r="P26" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
       <c r="S26" s="5"/>
@@ -2618,28 +2659,26 @@
       <c r="Z26" s="5"/>
       <c r="AA26" s="5"/>
       <c r="AB26" s="5"/>
-      <c r="AC26" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AD26" s="5" t="s">
-        <v>81</v>
-      </c>
+      <c r="AC26" s="5"/>
+      <c r="AD26" s="5"/>
       <c r="AE26" s="9"/>
     </row>
-    <row r="27" spans="2:31" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="23">
+    <row r="27" spans="2:31" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="22">
         <v>22</v>
       </c>
-      <c r="C27" s="15" t="s">
-        <v>17</v>
+      <c r="C27" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
+      <c r="H27" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -2661,39 +2700,31 @@
       <c r="AA27" s="5"/>
       <c r="AB27" s="5"/>
       <c r="AC27" s="5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="AD27" s="5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="AE27" s="9"/>
     </row>
-    <row r="28" spans="2:31" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="23">
+    <row r="28" spans="2:31" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="22">
         <v>23</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="18" t="s">
-        <v>88</v>
-      </c>
+      <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
@@ -2710,26 +2741,40 @@
       <c r="Z28" s="5"/>
       <c r="AA28" s="5"/>
       <c r="AB28" s="5"/>
-      <c r="AC28" s="5"/>
-      <c r="AD28" s="5"/>
+      <c r="AC28" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD28" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="AE28" s="9"/>
     </row>
     <row r="29" spans="2:31" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="23">
+      <c r="B29" s="22">
         <v>24</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>18</v>
+      <c r="C29" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+      <c r="E29" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
+      <c r="G29" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
+      <c r="L29" s="18" t="s">
+        <v>87</v>
+      </c>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
@@ -2746,141 +2791,129 @@
       <c r="Z29" s="5"/>
       <c r="AA29" s="5"/>
       <c r="AB29" s="5"/>
-      <c r="AC29" s="5" t="s">
-        <v>89</v>
-      </c>
+      <c r="AC29" s="5"/>
       <c r="AD29" s="5"/>
       <c r="AE29" s="9"/>
     </row>
-    <row r="30" spans="2:31" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="23">
+    <row r="30" spans="2:31" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="22">
         <v>25</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>65</v>
+      <c r="C30" s="15" t="s">
+        <v>18</v>
       </c>
       <c r="D30" s="5"/>
-      <c r="E30" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
-      <c r="L30" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="L30" s="5"/>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
-      <c r="S30" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="T30" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="U30" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="V30" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="W30" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="X30" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y30" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z30" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA30" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB30" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="W30" s="5"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="5"/>
+      <c r="AB30" s="5"/>
+      <c r="AC30" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="AD30" s="5"/>
       <c r="AE30" s="9"/>
     </row>
-    <row r="31" spans="2:31" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="23">
+    <row r="31" spans="2:31" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="22">
         <v>26</v>
       </c>
-      <c r="C31" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+      <c r="C31" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
+      <c r="L31" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
       <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
-      <c r="U31" s="5"/>
-      <c r="V31" s="5"/>
-      <c r="W31" s="5"/>
-      <c r="X31" s="5"/>
-      <c r="Y31" s="5"/>
-      <c r="Z31" s="5"/>
-      <c r="AA31" s="5"/>
-      <c r="AB31" s="5"/>
-      <c r="AC31" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD31" s="5" t="s">
-        <v>91</v>
-      </c>
+      <c r="S31" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="T31" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="U31" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="V31" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="W31" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="X31" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y31" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z31" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA31" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB31" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC31" s="5"/>
+      <c r="AD31" s="5"/>
       <c r="AE31" s="9"/>
     </row>
-    <row r="32" spans="2:31" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="23">
+    <row r="32" spans="2:31" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="22">
         <v>27</v>
       </c>
-      <c r="C32" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="C32" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
@@ -2894,41 +2927,41 @@
       <c r="T32" s="5"/>
       <c r="U32" s="5"/>
       <c r="V32" s="5"/>
-      <c r="W32" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="X32" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y32" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z32" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA32" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB32" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AC32" s="5"/>
-      <c r="AD32" s="5"/>
+      <c r="W32" s="5"/>
+      <c r="X32" s="5"/>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="5"/>
+      <c r="AB32" s="5"/>
+      <c r="AC32" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD32" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AE32" s="9"/>
     </row>
-    <row r="33" spans="2:31" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="23">
+    <row r="33" spans="2:31" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="22">
         <v>28</v>
       </c>
-      <c r="C33" s="15" t="s">
-        <v>20</v>
+      <c r="C33" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="E33" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
+      <c r="G33" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
@@ -2943,37 +2976,35 @@
       <c r="U33" s="5"/>
       <c r="V33" s="5"/>
       <c r="W33" s="5" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="X33" s="5" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="Y33" s="5" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="Z33" s="5" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="AA33" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB33" s="21" t="s">
-        <v>108</v>
+        <v>91</v>
+      </c>
+      <c r="AB33" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="AC33" s="5"/>
       <c r="AD33" s="5"/>
       <c r="AE33" s="9"/>
     </row>
-    <row r="34" spans="2:31" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="23">
+    <row r="34" spans="2:31" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="22">
         <v>29</v>
       </c>
-      <c r="C34" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>94</v>
-      </c>
+      <c r="C34" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
@@ -2992,41 +3023,43 @@
       <c r="T34" s="5"/>
       <c r="U34" s="5"/>
       <c r="V34" s="5"/>
-      <c r="W34" s="5"/>
-      <c r="X34" s="5"/>
-      <c r="Y34" s="5"/>
-      <c r="Z34" s="5"/>
-      <c r="AA34" s="5"/>
-      <c r="AB34" s="5"/>
-      <c r="AC34" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD34" s="5" t="s">
-        <v>94</v>
-      </c>
+      <c r="W34" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="X34" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y34" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z34" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA34" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB34" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC34" s="5"/>
+      <c r="AD34" s="5"/>
       <c r="AE34" s="9"/>
     </row>
-    <row r="35" spans="2:31" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="23">
+    <row r="35" spans="2:31" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="22">
         <v>30</v>
       </c>
-      <c r="C35" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="C35" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="5"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="H35" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="I35" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
@@ -3036,49 +3069,45 @@
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
       <c r="R35" s="5"/>
-      <c r="S35" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="T35" s="5" t="s">
-        <v>95</v>
-      </c>
+      <c r="S35" s="5"/>
+      <c r="T35" s="5"/>
       <c r="U35" s="5"/>
       <c r="V35" s="5"/>
-      <c r="W35" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="X35" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y35" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z35" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA35" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB35" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC35" s="5"/>
-      <c r="AD35" s="5"/>
+      <c r="W35" s="5"/>
+      <c r="X35" s="5"/>
+      <c r="Y35" s="5"/>
+      <c r="Z35" s="5"/>
+      <c r="AA35" s="5"/>
+      <c r="AB35" s="5"/>
+      <c r="AC35" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD35" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="AE35" s="9"/>
     </row>
-    <row r="36" spans="2:31" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="23">
+    <row r="36" spans="2:31" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="22">
         <v>31</v>
       </c>
-      <c r="C36" s="14" t="s">
-        <v>23</v>
+      <c r="C36" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
+      <c r="E36" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
+      <c r="G36" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
@@ -3089,33 +3118,43 @@
       <c r="Q36" s="5"/>
       <c r="R36" s="5"/>
       <c r="S36" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="T36" s="5" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="U36" s="5"/>
       <c r="V36" s="5"/>
-      <c r="W36" s="5"/>
-      <c r="X36" s="5"/>
-      <c r="Y36" s="5"/>
-      <c r="Z36" s="5"/>
-      <c r="AA36" s="5"/>
-      <c r="AB36" s="5"/>
+      <c r="W36" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="X36" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y36" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z36" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA36" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB36" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="AC36" s="5"/>
       <c r="AD36" s="5"/>
       <c r="AE36" s="9"/>
     </row>
-    <row r="37" spans="2:31" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="23">
+    <row r="37" spans="2:31" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="22">
         <v>32</v>
       </c>
-      <c r="C37" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>97</v>
-      </c>
+      <c r="C37" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
@@ -3130,8 +3169,12 @@
       <c r="P37" s="5"/>
       <c r="Q37" s="5"/>
       <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
+      <c r="S37" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="T37" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="U37" s="5"/>
       <c r="V37" s="5"/>
       <c r="W37" s="5"/>
@@ -3140,128 +3183,124 @@
       <c r="Z37" s="5"/>
       <c r="AA37" s="5"/>
       <c r="AB37" s="5"/>
-      <c r="AC37" s="5" t="s">
+      <c r="AC37" s="5"/>
+      <c r="AD37" s="5"/>
+      <c r="AE37" s="9"/>
+    </row>
+    <row r="38" spans="2:31" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="22">
+        <v>33</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="5"/>
+      <c r="U38" s="5"/>
+      <c r="V38" s="5"/>
+      <c r="W38" s="5"/>
+      <c r="X38" s="5"/>
+      <c r="Y38" s="5"/>
+      <c r="Z38" s="5"/>
+      <c r="AA38" s="5"/>
+      <c r="AB38" s="5"/>
+      <c r="AC38" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD38" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE38" s="9"/>
+    </row>
+    <row r="39" spans="2:31" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="22">
+        <v>34</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="7"/>
+      <c r="E39" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F39" s="7"/>
+      <c r="G39" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="T39" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="U39" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="AD37" s="5" t="s">
+      <c r="V39" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="AE37" s="9"/>
-    </row>
-    <row r="38" spans="2:31" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="23">
-        <v>33</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F38" s="7"/>
-      <c r="G38" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="H38" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="I38" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="7"/>
-      <c r="P38" s="7"/>
-      <c r="Q38" s="7"/>
-      <c r="R38" s="7"/>
-      <c r="S38" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="T38" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="U38" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="V38" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="W38" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="X38" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y38" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z38" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA38" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB38" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC38" s="7"/>
-      <c r="AD38" s="7"/>
-      <c r="AE38" s="10"/>
-    </row>
-    <row r="39" spans="2:31" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="23">
-        <v>34</v>
-      </c>
-      <c r="C39" s="15" t="s">
+      <c r="W39" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="X39" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y39" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z39" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA39" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB39" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC39" s="7"/>
+      <c r="AD39" s="7"/>
+      <c r="AE39" s="10"/>
+    </row>
+    <row r="40" spans="2:31" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="22">
+        <v>35</v>
+      </c>
+      <c r="C40" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5"/>
-      <c r="U39" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="V39" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="W39" s="5"/>
-      <c r="X39" s="5"/>
-      <c r="Y39" s="5"/>
-      <c r="Z39" s="5"/>
-      <c r="AA39" s="5"/>
-      <c r="AB39" s="5"/>
-      <c r="AC39" s="5"/>
-      <c r="AD39" s="5"/>
-      <c r="AE39" s="9"/>
-    </row>
-    <row r="40" spans="2:31" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="23">
-        <v>35</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>99</v>
-      </c>
+      <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
@@ -3278,47 +3317,37 @@
       <c r="R40" s="5"/>
       <c r="S40" s="5"/>
       <c r="T40" s="5"/>
-      <c r="U40" s="5"/>
-      <c r="V40" s="5"/>
+      <c r="U40" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="V40" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="W40" s="5"/>
       <c r="X40" s="5"/>
       <c r="Y40" s="5"/>
       <c r="Z40" s="5"/>
       <c r="AA40" s="5"/>
       <c r="AB40" s="5"/>
-      <c r="AC40" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="AD40" s="5" t="s">
-        <v>57</v>
-      </c>
+      <c r="AC40" s="5"/>
+      <c r="AD40" s="5"/>
       <c r="AE40" s="9"/>
     </row>
     <row r="41" spans="2:31" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="23">
+      <c r="B41" s="22">
         <v>36</v>
       </c>
-      <c r="C41" s="15" t="s">
-        <v>67</v>
+      <c r="C41" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>65</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
@@ -3328,57 +3357,49 @@
       <c r="P41" s="5"/>
       <c r="Q41" s="5"/>
       <c r="R41" s="5"/>
-      <c r="S41" s="5" t="s">
+      <c r="S41" s="5"/>
+      <c r="T41" s="5"/>
+      <c r="U41" s="5"/>
+      <c r="V41" s="5"/>
+      <c r="W41" s="5"/>
+      <c r="X41" s="5"/>
+      <c r="Y41" s="5"/>
+      <c r="Z41" s="5"/>
+      <c r="AA41" s="5"/>
+      <c r="AB41" s="5"/>
+      <c r="AC41" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD41" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE41" s="9"/>
+    </row>
+    <row r="42" spans="2:31" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="22">
+        <v>37</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="T41" s="5" t="s">
+      <c r="F42" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="U41" s="5" t="s">
+      <c r="G42" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="V41" s="5" t="s">
+      <c r="H42" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="W41" s="5" t="s">
+      <c r="I42" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="X41" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y41" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z41" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA41" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB41" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC41" s="5"/>
-      <c r="AD41" s="5"/>
-      <c r="AE41" s="9"/>
-    </row>
-    <row r="42" spans="2:31" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="23">
-        <v>37</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
@@ -3388,35 +3409,53 @@
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
       <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
-      <c r="U42" s="5"/>
-      <c r="V42" s="5"/>
-      <c r="W42" s="5"/>
-      <c r="X42" s="5"/>
-      <c r="Y42" s="5"/>
-      <c r="Z42" s="5"/>
-      <c r="AA42" s="5"/>
-      <c r="AB42" s="5"/>
-      <c r="AC42" s="5" t="s">
+      <c r="S42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="T42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="U42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="V42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="W42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="X42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC42" s="5"/>
+      <c r="AD42" s="5"/>
+      <c r="AE42" s="9"/>
+    </row>
+    <row r="43" spans="2:31" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="22">
+        <v>38</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AD42" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE42" s="9"/>
-    </row>
-    <row r="43" spans="2:31" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="23">
-        <v>38</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E43" s="5"/>
+      <c r="E43" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
@@ -3441,30 +3480,28 @@
       <c r="AA43" s="5"/>
       <c r="AB43" s="5"/>
       <c r="AC43" s="5" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="AD43" s="5" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="AE43" s="9"/>
     </row>
-    <row r="44" spans="2:31" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="23">
+    <row r="44" spans="2:31" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="22">
         <v>39</v>
       </c>
-      <c r="C44" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="C44" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
-      <c r="I44" s="5" t="s">
-        <v>103</v>
-      </c>
+      <c r="I44" s="5"/>
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
@@ -3484,9 +3521,53 @@
       <c r="Z44" s="5"/>
       <c r="AA44" s="5"/>
       <c r="AB44" s="5"/>
-      <c r="AC44" s="5"/>
-      <c r="AD44" s="5"/>
+      <c r="AC44" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD44" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="AE44" s="9"/>
+    </row>
+    <row r="45" spans="2:31" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="22">
+        <v>40</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="5"/>
+      <c r="U45" s="5"/>
+      <c r="V45" s="5"/>
+      <c r="W45" s="5"/>
+      <c r="X45" s="5"/>
+      <c r="Y45" s="5"/>
+      <c r="Z45" s="5"/>
+      <c r="AA45" s="5"/>
+      <c r="AB45" s="5"/>
+      <c r="AC45" s="5"/>
+      <c r="AD45" s="5"/>
+      <c r="AE45" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>